<commit_message>
Updated the network protocol
</commit_message>
<xml_diff>
--- a/Documentation/MCUnity Network Protocol.xlsx
+++ b/Documentation/MCUnity Network Protocol.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Packet Formats" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Operation</t>
   </si>
@@ -144,7 +144,25 @@
     <t>setup operations sequence</t>
   </si>
   <si>
-    <t>0x05</t>
+    <t>Forces the firmware to send the</t>
+  </si>
+  <si>
+    <t>Request int</t>
+  </si>
+  <si>
+    <t>current value of all int variables</t>
+  </si>
+  <si>
+    <t>&lt;reserved&gt;</t>
+  </si>
+  <si>
+    <t>value 1</t>
+  </si>
+  <si>
+    <t>value 2</t>
+  </si>
+  <si>
+    <t>(shown for 2 variables)</t>
   </si>
 </sst>
 </file>
@@ -179,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -216,19 +234,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -258,6 +302,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -540,26 +600,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AN17"/>
+  <dimension ref="B3:AN26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.86328125" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" customWidth="1"/>
     <col min="5" max="5" width="28.73046875" customWidth="1"/>
     <col min="6" max="6" width="9.06640625" style="1"/>
     <col min="7" max="7" width="5.59765625" style="2" customWidth="1"/>
-    <col min="8" max="17" width="5.59765625" style="3" customWidth="1"/>
+    <col min="8" max="17" width="5.59765625" style="15" customWidth="1"/>
     <col min="18" max="20" width="5.59765625" customWidth="1"/>
-    <col min="21" max="36" width="5.59765625" style="3" customWidth="1"/>
-    <col min="37" max="40" width="9.06640625" style="3"/>
+    <col min="21" max="36" width="5.59765625" style="15" customWidth="1"/>
+    <col min="37" max="40" width="9.06640625" style="15"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:40" x14ac:dyDescent="0.45">
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -567,333 +627,251 @@
       <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:40" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>1</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>2</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>3</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>4</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <v>5</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>6</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>7</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="8">
         <v>8</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>9</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="8">
         <v>10</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5" s="8">
         <v>11</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="8">
         <v>12</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="8">
         <v>13</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="8">
         <v>14</v>
       </c>
-      <c r="V5" s="9">
+      <c r="V5" s="8">
         <v>15</v>
       </c>
-      <c r="W5" s="9">
+      <c r="W5" s="8">
         <v>16</v>
       </c>
-      <c r="X5" s="9">
+      <c r="X5" s="8">
         <v>17</v>
       </c>
-      <c r="Y5" s="9">
+      <c r="Y5" s="8">
         <v>18</v>
       </c>
-      <c r="Z5" s="9">
+      <c r="Z5" s="8">
         <v>19</v>
       </c>
-      <c r="AA5" s="9">
+      <c r="AA5" s="8">
         <v>20</v>
       </c>
-      <c r="AB5" s="9">
+      <c r="AB5" s="8">
         <v>21</v>
       </c>
-      <c r="AC5" s="9">
+      <c r="AC5" s="8">
         <v>22</v>
       </c>
-      <c r="AD5" s="9">
+      <c r="AD5" s="8">
         <v>23</v>
       </c>
-      <c r="AE5" s="9">
+      <c r="AE5" s="8">
         <v>24</v>
       </c>
-      <c r="AF5" s="9">
+      <c r="AF5" s="8">
         <v>25</v>
       </c>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
     </row>
     <row r="6" spans="2:40" x14ac:dyDescent="0.45">
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:40" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
-      <c r="AG7" s="14"/>
-      <c r="AH7" s="14"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="14"/>
-      <c r="AK7" s="14"/>
-      <c r="AL7" s="14"/>
-      <c r="AM7" s="14"/>
-      <c r="AN7" s="14"/>
+    <row r="7" spans="2:40" s="19" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F7" s="20"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="21"/>
+      <c r="AI7" s="21"/>
+      <c r="AJ7" s="21"/>
+      <c r="AK7" s="21"/>
+      <c r="AL7" s="21"/>
+      <c r="AM7" s="21"/>
+      <c r="AN7" s="21"/>
     </row>
     <row r="8" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="G8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:40" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
-      <c r="AG9" s="14"/>
-      <c r="AH9" s="14"/>
-      <c r="AI9" s="14"/>
-      <c r="AJ9" s="14"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="14"/>
-      <c r="AN9" s="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
     </row>
     <row r="10" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="16"/>
-    </row>
-    <row r="11" spans="2:40" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="T11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="U11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD11" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="14"/>
-      <c r="AJ11" s="14"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
-      <c r="AN11" s="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
     </row>
     <row r="12" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -902,180 +880,409 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2">
-        <v>3</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="2:40" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="14"/>
-      <c r="AG13" s="14"/>
-      <c r="AH13" s="14"/>
-      <c r="AI13" s="14"/>
-      <c r="AJ13" s="14"/>
-      <c r="AK13" s="14"/>
-      <c r="AL13" s="14"/>
-      <c r="AM13" s="14"/>
-      <c r="AN13" s="14"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="E13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="13"/>
+      <c r="AI13" s="13"/>
+      <c r="AJ13" s="13"/>
+      <c r="AK13" s="13"/>
+      <c r="AL13" s="13"/>
+      <c r="AM13" s="13"/>
+      <c r="AN13" s="13"/>
     </row>
     <row r="14" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G14" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:40" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="14"/>
-      <c r="AG15" s="14"/>
-      <c r="AH15" s="14"/>
-      <c r="AI15" s="14"/>
-      <c r="AJ15" s="14"/>
-      <c r="AK15" s="14"/>
-      <c r="AL15" s="14"/>
-      <c r="AM15" s="14"/>
-      <c r="AN15" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:40" s="19" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F15" s="20"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="21"/>
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="21"/>
+      <c r="AC15" s="21"/>
+      <c r="AD15" s="21"/>
+      <c r="AE15" s="21"/>
+      <c r="AF15" s="21"/>
+      <c r="AG15" s="21"/>
+      <c r="AH15" s="21"/>
+      <c r="AI15" s="21"/>
+      <c r="AJ15" s="21"/>
+      <c r="AK15" s="21"/>
+      <c r="AL15" s="21"/>
+      <c r="AM15" s="21"/>
+      <c r="AN15" s="21"/>
     </row>
     <row r="16" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1">
+        <v>18</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+    </row>
+    <row r="17" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="U17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB17" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="13"/>
+      <c r="AK17" s="13"/>
+      <c r="AL17" s="13"/>
+      <c r="AM17" s="13"/>
+      <c r="AN17" s="13"/>
+    </row>
+    <row r="18" spans="2:40" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>11</v>
       </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2">
+        <v>5</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+    </row>
+    <row r="19" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="13"/>
+      <c r="AG19" s="13"/>
+      <c r="AH19" s="13"/>
+      <c r="AI19" s="13"/>
+      <c r="AJ19" s="13"/>
+      <c r="AK19" s="13"/>
+      <c r="AL19" s="13"/>
+      <c r="AM19" s="13"/>
+      <c r="AN19" s="13"/>
+    </row>
+    <row r="20" spans="2:40" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="2">
+        <v>6</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+    </row>
+    <row r="21" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="E21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
+      <c r="AD21" s="13"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
+      <c r="AH21" s="13"/>
+      <c r="AI21" s="13"/>
+      <c r="AJ21" s="13"/>
+      <c r="AK21" s="13"/>
+      <c r="AL21" s="13"/>
+      <c r="AM21" s="13"/>
+      <c r="AN21" s="13"/>
+    </row>
+    <row r="22" spans="2:40" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="5:40" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="E17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="14"/>
-      <c r="AF17" s="14"/>
-      <c r="AG17" s="14"/>
-      <c r="AH17" s="14"/>
-      <c r="AI17" s="14"/>
-      <c r="AJ17" s="14"/>
-      <c r="AK17" s="14"/>
-      <c r="AL17" s="14"/>
-      <c r="AM17" s="14"/>
-      <c r="AN17" s="14"/>
+      <c r="G22" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:40" s="19" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E23" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="21"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="21"/>
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
+      <c r="AE23" s="21"/>
+      <c r="AF23" s="21"/>
+      <c r="AG23" s="21"/>
+      <c r="AH23" s="21"/>
+      <c r="AI23" s="21"/>
+      <c r="AJ23" s="21"/>
+      <c r="AK23" s="21"/>
+      <c r="AL23" s="21"/>
+      <c r="AM23" s="21"/>
+      <c r="AN23" s="21"/>
+    </row>
+    <row r="24" spans="2:40" x14ac:dyDescent="0.45">
+      <c r="G24" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:40" x14ac:dyDescent="0.45">
+      <c r="G26" s="2">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="U10:X10"/>
-    <mergeCell ref="Y10:AF10"/>
+  <mergeCells count="8">
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="Q16:T16"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="Y16:AF16"/>
+    <mergeCell ref="I18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added "update int" operation.
</commit_message>
<xml_diff>
--- a/Documentation/MCUnity Network Protocol.xlsx
+++ b/Documentation/MCUnity Network Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Operation</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Setup GUI element for an "int"</t>
   </si>
   <si>
-    <t>Update all "int" GUI elements</t>
-  </si>
-  <si>
     <t>Setup int</t>
   </si>
   <si>
@@ -162,7 +159,13 @@
     <t>value 2</t>
   </si>
   <si>
-    <t>(shown for 2 variables)</t>
+    <t>Update some /all "int" GUI</t>
+  </si>
+  <si>
+    <t>elements (shown for 2 variables)</t>
+  </si>
+  <si>
+    <t>offset</t>
   </si>
 </sst>
 </file>
@@ -305,12 +308,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -318,6 +315,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,7 +606,7 @@
   <dimension ref="B3:AN26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -620,12 +623,12 @@
   <sheetData>
     <row r="3" spans="2:40" x14ac:dyDescent="0.45">
       <c r="J3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:40" x14ac:dyDescent="0.45">
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>4</v>
@@ -739,43 +742,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:40" s="19" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F7" s="20"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="21"/>
-      <c r="AL7" s="21"/>
-      <c r="AM7" s="21"/>
-      <c r="AN7" s="21"/>
+    <row r="7" spans="2:40" s="17" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F7" s="18"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="19"/>
+      <c r="AH7" s="19"/>
+      <c r="AI7" s="19"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="19"/>
+      <c r="AL7" s="19"/>
+      <c r="AM7" s="19"/>
+      <c r="AN7" s="19"/>
     </row>
     <row r="8" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
@@ -871,7 +874,7 @@
     </row>
     <row r="12" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -880,7 +883,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -891,7 +894,7 @@
     </row>
     <row r="13" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E13" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="10"/>
       <c r="AG13" s="13"/>
@@ -905,43 +908,43 @@
     </row>
     <row r="14" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:40" s="19" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F15" s="20"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="21"/>
-      <c r="AF15" s="21"/>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="21"/>
-      <c r="AI15" s="21"/>
-      <c r="AJ15" s="21"/>
-      <c r="AK15" s="21"/>
-      <c r="AL15" s="21"/>
-      <c r="AM15" s="21"/>
-      <c r="AN15" s="21"/>
+    <row r="15" spans="2:40" s="17" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F15" s="18"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="19"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="19"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
+      <c r="AL15" s="19"/>
+      <c r="AM15" s="19"/>
+      <c r="AN15" s="19"/>
     </row>
     <row r="16" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -959,99 +962,99 @@
         <v>4</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17" t="s">
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="17" t="s">
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="V16" s="17"/>
-      <c r="W16" s="17"/>
-      <c r="X16" s="17"/>
-      <c r="Y16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z16" s="17"/>
-      <c r="AA16" s="17"/>
-      <c r="AB16" s="17"/>
-      <c r="AC16" s="17"/>
-      <c r="AD16" s="17"/>
-      <c r="AE16" s="17"/>
-      <c r="AF16" s="17"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="23"/>
+      <c r="AB16" s="23"/>
+      <c r="AC16" s="23"/>
+      <c r="AD16" s="23"/>
+      <c r="AE16" s="23"/>
+      <c r="AF16" s="23"/>
     </row>
     <row r="17" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
       <c r="H17" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="T17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T17" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="U17" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V17" s="13"/>
       <c r="W17" s="13"/>
       <c r="X17" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="Z17" s="14" t="s">
+      <c r="AA17" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AA17" s="14" t="s">
+      <c r="AB17" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AB17" s="14" t="s">
+      <c r="AC17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="AC17" s="14" t="s">
+      <c r="AD17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AD17" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="AE17" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AF17" s="13"/>
       <c r="AG17" s="13"/>
@@ -1065,7 +1068,7 @@
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1083,28 +1086,28 @@
         <v>5</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
     </row>
     <row r="19" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
       <c r="H19" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
@@ -1134,7 +1137,7 @@
     </row>
     <row r="20" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -1143,23 +1146,26 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="G20" s="2">
         <v>6</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
     </row>
     <row r="21" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E21" s="9" t="s">
@@ -1167,23 +1173,25 @@
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="13"/>
+      <c r="H21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="J21" s="13"/>
-      <c r="K21" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="K21" s="13"/>
       <c r="L21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="M21" s="13"/>
+      <c r="M21" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="N21" s="13"/>
-      <c r="O21" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="P21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="Q21" s="13"/>
       <c r="U21" s="13"/>
       <c r="V21" s="13"/>
@@ -1208,7 +1216,7 @@
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1217,7 +1225,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1226,42 +1234,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:40" s="19" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E23" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="21"/>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
-      <c r="Y23" s="21"/>
-      <c r="Z23" s="21"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="21"/>
-      <c r="AE23" s="21"/>
-      <c r="AF23" s="21"/>
-      <c r="AG23" s="21"/>
-      <c r="AH23" s="21"/>
-      <c r="AI23" s="21"/>
-      <c r="AJ23" s="21"/>
-      <c r="AK23" s="21"/>
-      <c r="AL23" s="21"/>
-      <c r="AM23" s="21"/>
-      <c r="AN23" s="21"/>
+    <row r="23" spans="2:40" s="17" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E23" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="19"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19"/>
+      <c r="AF23" s="19"/>
+      <c r="AG23" s="19"/>
+      <c r="AH23" s="19"/>
+      <c r="AI23" s="19"/>
+      <c r="AJ23" s="19"/>
+      <c r="AK23" s="19"/>
+      <c r="AL23" s="19"/>
+      <c r="AM23" s="19"/>
+      <c r="AN23" s="19"/>
     </row>
     <row r="24" spans="2:40" x14ac:dyDescent="0.45">
       <c r="G24" s="2">
@@ -1275,14 +1283,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="Y16:AF16"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="M20:P20"/>
     <mergeCell ref="I16:L16"/>
     <mergeCell ref="M16:P16"/>
     <mergeCell ref="Q16:T16"/>
-    <mergeCell ref="U16:X16"/>
-    <mergeCell ref="Y16:AF16"/>
-    <mergeCell ref="I18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added support for new MCUnity operations, notably remote-calling functions of the firmware.
</commit_message>
<xml_diff>
--- a/Documentation/MCUnity Network Protocol.xlsx
+++ b/Documentation/MCUnity Network Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>Operation</t>
   </si>
@@ -166,6 +166,57 @@
   </si>
   <si>
     <t>offset</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>Setup function</t>
+  </si>
+  <si>
+    <t>Call function</t>
+  </si>
+  <si>
+    <t>Setup GUI element for a firmware</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call a firmware function </t>
   </si>
 </sst>
 </file>
@@ -200,7 +251,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -266,19 +317,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,9 +346,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -314,13 +365,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AN26"/>
+  <dimension ref="B3:AN31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -614,15 +690,15 @@
     <col min="2" max="2" width="12.19921875" customWidth="1"/>
     <col min="5" max="5" width="28.73046875" customWidth="1"/>
     <col min="6" max="6" width="9.06640625" style="1"/>
-    <col min="7" max="7" width="5.59765625" style="2" customWidth="1"/>
-    <col min="8" max="17" width="5.59765625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="5.59765625" style="20" customWidth="1"/>
+    <col min="8" max="17" width="5.59765625" style="12" customWidth="1"/>
     <col min="18" max="20" width="5.59765625" customWidth="1"/>
-    <col min="21" max="36" width="5.59765625" style="15" customWidth="1"/>
-    <col min="37" max="40" width="9.06640625" style="15"/>
+    <col min="21" max="36" width="5.59765625" style="12" customWidth="1"/>
+    <col min="37" max="40" width="9.06640625" style="12"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:40" x14ac:dyDescent="0.45">
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -630,193 +706,234 @@
       <c r="F4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:40" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:40" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="20">
         <v>0</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <v>1</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="6">
         <v>2</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="6">
         <v>3</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="6">
         <v>4</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <v>5</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="6">
         <v>6</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="6">
         <v>7</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="6">
         <v>8</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="6">
         <v>9</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="6">
         <v>10</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="6">
         <v>11</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5" s="6">
         <v>12</v>
       </c>
-      <c r="T5" s="8">
+      <c r="T5" s="6">
         <v>13</v>
       </c>
-      <c r="U5" s="8">
+      <c r="U5" s="6">
         <v>14</v>
       </c>
-      <c r="V5" s="8">
+      <c r="V5" s="6">
         <v>15</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W5" s="6">
         <v>16</v>
       </c>
-      <c r="X5" s="8">
+      <c r="X5" s="6">
         <v>17</v>
       </c>
-      <c r="Y5" s="8">
+      <c r="Y5" s="6">
         <v>18</v>
       </c>
-      <c r="Z5" s="8">
+      <c r="Z5" s="6">
         <v>19</v>
       </c>
-      <c r="AA5" s="8">
+      <c r="AA5" s="6">
         <v>20</v>
       </c>
-      <c r="AB5" s="8">
+      <c r="AB5" s="6">
         <v>21</v>
       </c>
-      <c r="AC5" s="8">
+      <c r="AC5" s="6">
         <v>22</v>
       </c>
-      <c r="AD5" s="8">
+      <c r="AD5" s="6">
         <v>23</v>
       </c>
-      <c r="AE5" s="8">
+      <c r="AE5" s="6">
         <v>24</v>
       </c>
-      <c r="AF5" s="8">
+      <c r="AF5" s="6">
         <v>25</v>
       </c>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8"/>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="8"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
     </row>
     <row r="6" spans="2:40" x14ac:dyDescent="0.45">
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:40" s="17" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F7" s="18"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="19"/>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="19"/>
-      <c r="AH7" s="19"/>
-      <c r="AI7" s="19"/>
-      <c r="AJ7" s="19"/>
-      <c r="AK7" s="19"/>
-      <c r="AL7" s="19"/>
-      <c r="AM7" s="19"/>
-      <c r="AN7" s="19"/>
+    <row r="7" spans="2:40" s="14" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F7" s="15"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="16"/>
+      <c r="AH7" s="16"/>
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+      <c r="AK7" s="16"/>
+      <c r="AL7" s="16"/>
+      <c r="AM7" s="16"/>
+      <c r="AN7" s="16"/>
     </row>
     <row r="8" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="13"/>
-      <c r="AJ9" s="13"/>
-      <c r="AK9" s="13"/>
-      <c r="AL9" s="13"/>
-      <c r="AM9" s="13"/>
-      <c r="AN9" s="13"/>
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="30"/>
+    </row>
+    <row r="9" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="E9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="10"/>
+      <c r="AK9" s="10"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="10"/>
     </row>
     <row r="10" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
@@ -834,43 +951,43 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="13"/>
-      <c r="AJ11" s="13"/>
-      <c r="AK11" s="13"/>
-      <c r="AL11" s="13"/>
-      <c r="AM11" s="13"/>
-      <c r="AN11" s="13"/>
+      <c r="G10" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F11" s="8"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="10"/>
+      <c r="AI11" s="10"/>
+      <c r="AJ11" s="10"/>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="10"/>
     </row>
     <row r="12" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
@@ -888,59 +1005,79 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="E13" s="9" t="s">
+      <c r="G12" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="E13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="13"/>
-      <c r="AI13" s="13"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="13"/>
-      <c r="AL13" s="13"/>
-      <c r="AM13" s="13"/>
-      <c r="AN13" s="13"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="24"/>
+      <c r="AG13" s="10"/>
+      <c r="AH13" s="10"/>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="10"/>
+      <c r="AK13" s="10"/>
+      <c r="AL13" s="10"/>
+      <c r="AM13" s="10"/>
+      <c r="AN13" s="10"/>
     </row>
     <row r="14" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:40" s="17" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F15" s="18"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19"/>
-      <c r="AC15" s="19"/>
-      <c r="AD15" s="19"/>
-      <c r="AE15" s="19"/>
-      <c r="AF15" s="19"/>
-      <c r="AG15" s="19"/>
-      <c r="AH15" s="19"/>
-      <c r="AI15" s="19"/>
-      <c r="AJ15" s="19"/>
-      <c r="AK15" s="19"/>
-      <c r="AL15" s="19"/>
-      <c r="AM15" s="19"/>
-      <c r="AN15" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:40" s="14" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F15" s="15"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="16"/>
+      <c r="AG15" s="16"/>
+      <c r="AH15" s="16"/>
+      <c r="AI15" s="16"/>
+      <c r="AJ15" s="16"/>
+      <c r="AK15" s="16"/>
+      <c r="AL15" s="16"/>
+      <c r="AM15" s="16"/>
+      <c r="AN15" s="16"/>
     </row>
     <row r="16" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
@@ -958,113 +1095,113 @@
       <c r="F16" s="1">
         <v>18</v>
       </c>
-      <c r="G16" s="2">
-        <v>4</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="G16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23" t="s">
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23" t="s">
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23" t="s">
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23" t="s">
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="23"/>
-    </row>
-    <row r="17" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12" t="s">
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+    </row>
+    <row r="17" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F17" s="8"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13" t="s">
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M17" s="13" t="s">
+      <c r="M17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13" t="s">
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q17" s="13" t="s">
+      <c r="Q17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="T17" s="9" t="s">
+      <c r="T17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="U17" s="13" t="s">
+      <c r="U17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13" t="s">
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Y17" s="14" t="s">
+      <c r="Y17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="Z17" s="14" t="s">
+      <c r="Z17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AA17" s="14" t="s">
+      <c r="AA17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AB17" s="14" t="s">
+      <c r="AB17" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AC17" s="14" t="s">
+      <c r="AC17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AD17" s="14" t="s">
+      <c r="AD17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AE17" s="14" t="s">
+      <c r="AE17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="13"/>
-      <c r="AM17" s="13"/>
-      <c r="AN17" s="13"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="10"/>
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
@@ -1082,58 +1219,58 @@
       <c r="F18" s="1">
         <v>6</v>
       </c>
-      <c r="G18" s="2">
-        <v>5</v>
-      </c>
-      <c r="H18" s="15" t="s">
+      <c r="G18" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="13" t="s">
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F19" s="8"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13" t="s">
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="13"/>
-      <c r="AD19" s="13"/>
-      <c r="AE19" s="13"/>
-      <c r="AF19" s="13"/>
-      <c r="AG19" s="13"/>
-      <c r="AH19" s="13"/>
-      <c r="AI19" s="13"/>
-      <c r="AJ19" s="13"/>
-      <c r="AK19" s="13"/>
-      <c r="AL19" s="13"/>
-      <c r="AM19" s="13"/>
-      <c r="AN19" s="13"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="10"/>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="10"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="10"/>
     </row>
     <row r="20" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
@@ -1148,71 +1285,71 @@
       <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="2">
-        <v>6</v>
-      </c>
-      <c r="H20" s="15" t="s">
+      <c r="G20" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22" t="s">
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-    </row>
-    <row r="21" spans="2:40" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="E21" s="9" t="s">
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+    </row>
+    <row r="21" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="E21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="9" t="s">
+      <c r="F21" s="8"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13" t="s">
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="M21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13" t="s">
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
-      <c r="AB21" s="13"/>
-      <c r="AC21" s="13"/>
-      <c r="AD21" s="13"/>
-      <c r="AE21" s="13"/>
-      <c r="AF21" s="13"/>
-      <c r="AG21" s="13"/>
-      <c r="AH21" s="13"/>
-      <c r="AI21" s="13"/>
-      <c r="AJ21" s="13"/>
-      <c r="AK21" s="13"/>
-      <c r="AL21" s="13"/>
-      <c r="AM21" s="13"/>
-      <c r="AN21" s="13"/>
+      <c r="Q21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="10"/>
+      <c r="AJ21" s="10"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="10"/>
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
@@ -1224,65 +1361,255 @@
       <c r="D22" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
-      <c r="G22" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:40" s="17" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E23" s="20" t="s">
+      <c r="G22" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:40" s="14" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E23" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="19"/>
-      <c r="AH23" s="19"/>
-      <c r="AI23" s="19"/>
-      <c r="AJ23" s="19"/>
-      <c r="AK23" s="19"/>
-      <c r="AL23" s="19"/>
-      <c r="AM23" s="19"/>
-      <c r="AN23" s="19"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="16"/>
+      <c r="AC23" s="16"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="16"/>
+      <c r="AG23" s="16"/>
+      <c r="AH23" s="16"/>
+      <c r="AI23" s="16"/>
+      <c r="AJ23" s="16"/>
+      <c r="AK23" s="16"/>
+      <c r="AL23" s="16"/>
+      <c r="AM23" s="16"/>
+      <c r="AN23" s="16"/>
     </row>
     <row r="24" spans="2:40" x14ac:dyDescent="0.45">
-      <c r="G24" s="2">
-        <v>8</v>
-      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F25" s="8"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
+      <c r="AD25" s="10"/>
+      <c r="AE25" s="10"/>
+      <c r="AF25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AH25" s="10"/>
+      <c r="AI25" s="10"/>
+      <c r="AJ25" s="10"/>
+      <c r="AK25" s="10"/>
+      <c r="AL25" s="10"/>
+      <c r="AM25" s="10"/>
+      <c r="AN25" s="10"/>
     </row>
     <row r="26" spans="2:40" x14ac:dyDescent="0.45">
-      <c r="G26" s="2">
-        <v>9</v>
-      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F27" s="8"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="10"/>
+      <c r="AE27" s="10"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="10"/>
+      <c r="AJ27" s="10"/>
+      <c r="AK27" s="10"/>
+      <c r="AL27" s="10"/>
+      <c r="AM27" s="10"/>
+      <c r="AN27" s="10"/>
+    </row>
+    <row r="28" spans="2:40" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F29" s="8"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="10"/>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="10"/>
+      <c r="AD29" s="10"/>
+      <c r="AE29" s="10"/>
+      <c r="AF29" s="10"/>
+      <c r="AG29" s="10"/>
+      <c r="AH29" s="10"/>
+      <c r="AI29" s="10"/>
+      <c r="AJ29" s="10"/>
+      <c r="AK29" s="10"/>
+      <c r="AL29" s="10"/>
+      <c r="AM29" s="10"/>
+      <c r="AN29" s="10"/>
+    </row>
+    <row r="30" spans="2:40" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="28"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="28"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="28"/>
+      <c r="AD30" s="28"/>
+      <c r="AE30" s="28"/>
+      <c r="AF30" s="28"/>
+      <c r="AG30" s="28"/>
+      <c r="AH30" s="28"/>
+      <c r="AI30" s="28"/>
+      <c r="AJ30" s="28"/>
+      <c r="AK30" s="28"/>
+      <c r="AL30" s="28"/>
+      <c r="AM30" s="28"/>
+      <c r="AN30" s="28"/>
+    </row>
+    <row r="31" spans="2:40" s="14" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F31" s="15"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="16"/>
+      <c r="Y31" s="16"/>
+      <c r="Z31" s="16"/>
+      <c r="AA31" s="16"/>
+      <c r="AB31" s="16"/>
+      <c r="AC31" s="16"/>
+      <c r="AD31" s="16"/>
+      <c r="AE31" s="16"/>
+      <c r="AF31" s="16"/>
+      <c r="AG31" s="16"/>
+      <c r="AH31" s="16"/>
+      <c r="AI31" s="16"/>
+      <c r="AJ31" s="16"/>
+      <c r="AK31" s="16"/>
+      <c r="AL31" s="16"/>
+      <c r="AM31" s="16"/>
+      <c r="AN31" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="I8:O8"/>
     <mergeCell ref="U16:X16"/>
     <mergeCell ref="Y16:AF16"/>
     <mergeCell ref="I18:L18"/>

</xml_diff>

<commit_message>
Reworked the GUI to support a tile-based paradigm
</commit_message>
<xml_diff>
--- a/Documentation/MCUnity Network Protocol.xlsx
+++ b/Documentation/MCUnity Network Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Operation</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t xml:space="preserve">Call a firmware function </t>
+  </si>
+  <si>
+    <t>Setup the display name of the MCU</t>
+  </si>
+  <si>
+    <t>running the firmware</t>
+  </si>
+  <si>
+    <t>TO DO</t>
   </si>
 </sst>
 </file>
@@ -243,12 +252,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -365,12 +380,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -395,10 +404,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AN31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -690,7 +703,7 @@
     <col min="2" max="2" width="12.19921875" customWidth="1"/>
     <col min="5" max="5" width="28.73046875" customWidth="1"/>
     <col min="6" max="6" width="9.06640625" style="1"/>
-    <col min="7" max="7" width="5.59765625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="5.59765625" style="18" customWidth="1"/>
     <col min="8" max="17" width="5.59765625" style="12" customWidth="1"/>
     <col min="18" max="20" width="5.59765625" customWidth="1"/>
     <col min="21" max="36" width="5.59765625" style="12" customWidth="1"/>
@@ -706,7 +719,7 @@
       <c r="F4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -726,7 +739,7 @@
       <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="18">
         <v>0</v>
       </c>
       <c r="H5" s="6">
@@ -820,7 +833,7 @@
     </row>
     <row r="7" spans="2:40" s="14" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F7" s="15"/>
-      <c r="G7" s="22"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
@@ -865,55 +878,69 @@
       <c r="E8" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="18" t="s">
         <v>49</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="30"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
     </row>
     <row r="9" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E9" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="N9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="O9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="P9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="Q9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="R9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="S9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -951,13 +978,13 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F11" s="8"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="21"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -1005,7 +1032,7 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="18" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1014,7 +1041,7 @@
         <v>39</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="22"/>
       <c r="AG13" s="10"/>
       <c r="AH13" s="10"/>
       <c r="AI13" s="10"/>
@@ -1040,7 +1067,7 @@
       <c r="F14" s="1">
         <v>2</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="18" t="s">
         <v>52</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1049,8 +1076,8 @@
     </row>
     <row r="15" spans="2:40" s="14" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F15" s="15"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="29" t="s">
+      <c r="G15" s="23"/>
+      <c r="H15" s="27" t="s">
         <v>21</v>
       </c>
       <c r="M15" s="16"/>
@@ -1095,50 +1122,50 @@
       <c r="F16" s="1">
         <v>18</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="18" t="s">
         <v>53</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18" t="s">
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18" t="s">
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18" t="s">
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18" t="s">
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
     </row>
     <row r="17" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F17" s="8"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="9" t="s">
         <v>21</v>
       </c>
@@ -1219,22 +1246,22 @@
       <c r="F18" s="1">
         <v>6</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="18" t="s">
         <v>54</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
     </row>
     <row r="19" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F19" s="8"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="21"/>
       <c r="H19" s="10" t="s">
         <v>21</v>
       </c>
@@ -1285,31 +1312,34 @@
       <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>55</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19" t="s">
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
     </row>
     <row r="21" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="E21" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="8"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="7" t="s">
         <v>21</v>
       </c>
@@ -1367,7 +1397,7 @@
       <c r="F22" s="1">
         <v>1</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="18" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1376,7 +1406,7 @@
         <v>42</v>
       </c>
       <c r="F23" s="15"/>
-      <c r="G23" s="22"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
@@ -1412,23 +1442,66 @@
       <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="E24" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="18" t="s">
         <v>57</v>
       </c>
+      <c r="H24" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
     </row>
     <row r="25" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F25" s="8"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="10"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
+      <c r="K25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
@@ -1454,13 +1527,13 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="18" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F27" s="8"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="21"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
@@ -1496,13 +1569,13 @@
       <c r="B28" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="2:40" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F29" s="8"/>
-      <c r="G29" s="23"/>
+      <c r="G29" s="21"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -1534,48 +1607,48 @@
       <c r="AM29" s="10"/>
       <c r="AN29" s="10"/>
     </row>
-    <row r="30" spans="2:40" s="26" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:40" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>43</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="28"/>
-      <c r="U30" s="28"/>
-      <c r="V30" s="28"/>
-      <c r="W30" s="28"/>
-      <c r="X30" s="28"/>
-      <c r="Y30" s="28"/>
-      <c r="Z30" s="28"/>
-      <c r="AA30" s="28"/>
-      <c r="AB30" s="28"/>
-      <c r="AC30" s="28"/>
-      <c r="AD30" s="28"/>
-      <c r="AE30" s="28"/>
-      <c r="AF30" s="28"/>
-      <c r="AG30" s="28"/>
-      <c r="AH30" s="28"/>
-      <c r="AI30" s="28"/>
-      <c r="AJ30" s="28"/>
-      <c r="AK30" s="28"/>
-      <c r="AL30" s="28"/>
-      <c r="AM30" s="28"/>
-      <c r="AN30" s="28"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="26"/>
+      <c r="AD30" s="26"/>
+      <c r="AE30" s="26"/>
+      <c r="AF30" s="26"/>
+      <c r="AG30" s="26"/>
+      <c r="AH30" s="26"/>
+      <c r="AI30" s="26"/>
+      <c r="AJ30" s="26"/>
+      <c r="AK30" s="26"/>
+      <c r="AL30" s="26"/>
+      <c r="AM30" s="26"/>
+      <c r="AN30" s="26"/>
     </row>
     <row r="31" spans="2:40" s="14" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F31" s="15"/>
-      <c r="G31" s="22"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
       <c r="J31" s="16"/>
@@ -1608,8 +1681,9 @@
       <c r="AN31" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="I8:O8"/>
+  <mergeCells count="10">
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="H24:K24"/>
     <mergeCell ref="U16:X16"/>
     <mergeCell ref="Y16:AF16"/>
     <mergeCell ref="I18:L18"/>

</xml_diff>